<commit_message>
Updates Facility Issues Excel Template
</commit_message>
<xml_diff>
--- a/print_docs/excel/excel_template/Facility Issue to Service Point.xlsx
+++ b/print_docs/excel/excel_template/Facility Issue to Service Point.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Service Point</t>
   </si>
@@ -30,39 +30,6 @@
     <t>Issue Quantity (Packs)</t>
   </si>
   <si>
-    <t>CCC</t>
-  </si>
-  <si>
-    <t>Pharmacy</t>
-  </si>
-  <si>
-    <t>Lab</t>
-  </si>
-  <si>
-    <t>Maternity</t>
-  </si>
-  <si>
-    <t>Injection Room</t>
-  </si>
-  <si>
-    <t>Dressing Room</t>
-  </si>
-  <si>
-    <t>TB Clinic</t>
-  </si>
-  <si>
-    <t>MCH</t>
-  </si>
-  <si>
-    <t>Diabetic Clinic</t>
-  </si>
-  <si>
-    <t>Youth Friendly Services</t>
-  </si>
-  <si>
-    <t>Outreach</t>
-  </si>
-  <si>
     <t>QUANTITY (PACKS)</t>
   </si>
   <si>
@@ -72,9 +39,6 @@
     <t>FACILITY ISSUE COMMODITIES TO SERVICE POINTS</t>
   </si>
   <si>
-    <t xml:space="preserve">Issue Date </t>
-  </si>
-  <si>
     <t>BATCH NUMBER</t>
   </si>
   <si>
@@ -91,12 +55,21 @@
   </si>
   <si>
     <t>HEALTH COMMODITIES MANAGEMENT PLATFORM (HCMP)</t>
+  </si>
+  <si>
+    <t>Issue Date (dd/mm/yyyy)</t>
+  </si>
+  <si>
+    <t>SERVICE POINT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -267,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -285,34 +258,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -324,13 +279,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,35 +613,38 @@
   <dimension ref="A1:S3062"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28" style="3" customWidth="1"/>
     <col min="2" max="2" width="28.5546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="32.88671875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="32.88671875" style="27" customWidth="1"/>
     <col min="4" max="4" width="39.6640625" style="5" customWidth="1"/>
     <col min="5" max="5" width="35" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="20"/>
+    <row r="1" spans="1:19" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="21"/>
+      <c r="A3" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="16"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -683,13 +661,13 @@
       <c r="S3" s="2"/>
     </row>
     <row r="4" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="23"/>
+      <c r="A4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="18"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -706,13 +684,13 @@
       <c r="S4" s="11"/>
     </row>
     <row r="5" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="23"/>
+      <c r="A5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="18"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -729,13 +707,13 @@
       <c r="S5" s="11"/>
     </row>
     <row r="6" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="23"/>
+      <c r="A6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="18"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
@@ -752,11 +730,11 @@
       <c r="S6" s="11"/>
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="23"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -773,13 +751,13 @@
       <c r="S7" s="11"/>
     </row>
     <row r="8" spans="1:19" s="1" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="29"/>
+      <c r="A8" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="34"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -796,39 +774,41 @@
       <c r="S8" s="2"/>
     </row>
     <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="31" t="s">
+      <c r="C9" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3062" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3062" s="7"/>
       <c r="B3062" s="8"/>
-      <c r="C3062" s="9"/>
+      <c r="C3062" s="26"/>
       <c r="D3062" s="9"/>
       <c r="E3062" s="10"/>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <mergeCells count="3">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A8:E8"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D1048576 E10:E1048576">
       <formula1>0</formula1>
     </dataValidation>
+    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C1048576"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -837,10 +817,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -848,58 +828,8 @@
     <col min="1" max="1" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -913,7 +843,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -924,13 +854,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>